<commit_message>
geek learning week1-2 homework
</commit_message>
<xml_diff>
--- a/src/cn/geek/git/main/week1/MemoryRef.xlsx
+++ b/src/cn/geek/git/main/week1/MemoryRef.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>最大堆内存</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;---------Xms------&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;------Xmn------&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,6 +81,33 @@
   </si>
   <si>
     <t>&lt;--Xss--&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1024m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>614m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;---Xms----&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eclipse为例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>132,751,360 个字节</t>
+  </si>
+  <si>
+    <t>4194304字节</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -92,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +125,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -128,9 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -160,8 +194,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>602</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>407</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>162332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1077,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1094,7 +1128,7 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.15">
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>13</v>
@@ -1102,48 +1136,64 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="14.25" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1151,15 +1201,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F17:G17"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>